<commit_message>
Made changes to the file
</commit_message>
<xml_diff>
--- a/Time&QualityWorkFlow.xlsx
+++ b/Time&QualityWorkFlow.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTOG\DANLC Lab Solution\Anudip-Lab-Solution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609FFB27-2978-41EA-ACC8-486AE2827E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C87040-104C-40F7-947D-79E40E9402D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,6 +69,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -76,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="139">
   <si>
     <t>Day 1</t>
   </si>
@@ -381,6 +383,9 @@
     <t>Average Quality</t>
   </si>
   <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
     <t>Day1</t>
   </si>
   <si>
@@ -429,99 +434,75 @@
     <t>Avg 1to 15</t>
   </si>
   <si>
+    <t xml:space="preserve">Did anyone take more time on Day 15 than Day 14? </t>
+  </si>
+  <si>
     <t>Ans=&gt;NO</t>
   </si>
   <si>
+    <t xml:space="preserve">Did anyone take longer because they were focusing too much on the quality? </t>
+  </si>
+  <si>
     <t>Ans=&gt; Dhruti decrease Quality &amp; Biju &amp; Harshita Increase Quality</t>
   </si>
   <si>
+    <t>How many have shown improvement in terms of TPT on Day 15</t>
+  </si>
+  <si>
     <t>Ans=&gt;Anand,Nupur,Biju,Gopal,Dhanya,Dipa improve quality in Day 15</t>
   </si>
   <si>
+    <t xml:space="preserve">Who are the top 3 members with the lowest TPT on the 15th Day </t>
+  </si>
+  <si>
     <t xml:space="preserve">Ans=&gt;Anushka,Arohi,Firoza members with the lowest TPT on the 15th Day  </t>
   </si>
   <si>
+    <t>who are the top 3 members with the lowest average TPT against day 1 to day 15? Are they the same person?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ans=&gt;Anushka,Arohi,Firoza members with the lowest TPT  against day 1 to  Day 15 </t>
   </si>
   <si>
+    <t>Which charts would give insights for each of the above points?</t>
+  </si>
+  <si>
     <t>Ans=&gt;Line Chart &amp; Column Chart</t>
   </si>
   <si>
-    <t>Ans=&gt;</t>
-  </si>
-  <si>
-    <t>Yes, the average TPT over the last 15 days is 1.867 seconds, which is an improvement compared to the overall average TPT of 1.885 seconds.</t>
-  </si>
-  <si>
-    <t>Yes, the standard deviation of TPT over the last 15 days is 0.150, which is lower than the overall standard deviation of 0.161. This indicates a decrease in variability, meaning the TPT has become more consistent.</t>
-  </si>
-  <si>
-    <t>Yes, the average TPT appears to be gradually decreasing over time from around 2.15.</t>
-  </si>
-  <si>
-    <t>To reduce the TPT further to 1.8, actions such as process optimization, workload balancing, and possibly automation of certain repetitive tasks might be necessary. Additional training or resources could also help to speed up the processes without sacrificing quality.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q1. Did anyone take more time on Day 15 than Day 14? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q2. Did anyone take longer because they were focusing too much on the quality? </t>
-  </si>
-  <si>
-    <t>Q3. How many have shown improvement in terms of TPT on Day 15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q4A. Who are the top 3 members with the lowest TPT on the 15th Day </t>
-  </si>
-  <si>
-    <t>Q4B. Who are the top 3 members with the lowest average TPT against day 1 to day 15? Are they the same person?</t>
-  </si>
-  <si>
-    <t>Q5. Which charts would give insights for each of the above points?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q6. What is the average of TPT against each day? </t>
-  </si>
-  <si>
-    <t>Q1. Did the average TPT improve?</t>
-  </si>
-  <si>
-    <t>Q2. Did the standard deviation decrease over the last 15 days?</t>
-  </si>
-  <si>
-    <t>Q3. Did the average TPT come down from the earlier TPT as your supervisor had indicated? What further actions may be required to bring down the average TPT to 1.8?</t>
-  </si>
-  <si>
-    <t>Q4. What insight would you share on the quality outcomes?</t>
-  </si>
-  <si>
-    <t>Consistency in Time Management: It seems that the time taken did not increase from Day 14 to Day 15, indicating stable process management.</t>
-  </si>
-  <si>
-    <t>Quality vs. Speed Trade-off: Some individuals like Dhruti reduced quality, while others like Biju and Harshit may have taken more time due to focusing on quality. This suggests a potential trade-off between speed and quality that needs to be managed carefully.</t>
+    <t xml:space="preserve">What is the average of TPT against each day? </t>
+  </si>
+  <si>
+    <t>Did the average TPT improve?</t>
+  </si>
+  <si>
+    <t>Ans=&gt;NO,Average TPT Decresed</t>
+  </si>
+  <si>
+    <t>Did the standard deviation decrease over the last 15 days?</t>
+  </si>
+  <si>
+    <t>Ans=&gt;Yes,standard deviation decrease over the last 15 days</t>
+  </si>
+  <si>
+    <t>Did the average TPT come down from the earlier TPT as your supervisor had indicated? What further actions may be required to bring down the average TPT to 1.8?</t>
+  </si>
+  <si>
+    <t>Ans=&gt; Average TPT Already 1.8.  no  further actions may be required to bring down the average TPT to 1.8</t>
+  </si>
+  <si>
+    <t>What insight would you share on the quality outcomes?</t>
+  </si>
+  <si>
+    <t>ANS=&gt; Day 1 to Day 15 Average Quality Increased</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="9">
+  <fonts count="6">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -533,14 +514,15 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -553,21 +535,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -675,37 +649,42 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1050,13 +1029,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>114935</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1103,13 +1082,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1156,13 +1135,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1241,6 +1220,59 @@
         <a:xfrm>
           <a:off x="1193800" y="809625"/>
           <a:ext cx="10893425" cy="6124575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="952500"/>
+          <a:ext cx="13011150" cy="7315200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1517,7 +1549,7 @@
   <dimension ref="A1:BI37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8350,14 +8382,14 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="13" t="s">
-        <v>134</v>
+      <c r="A1" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -8368,87 +8400,345 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="13" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:22">
-      <c r="A1" s="13" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22">
-      <c r="A3" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="5" spans="1:4" ht="15.75">
+      <c r="A5" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="1">
+        <f>AVERAGE(tptday1)</f>
+        <v>2.1506866285714299</v>
+      </c>
+      <c r="C6" s="1">
+        <f>AVERAGE(tptq1)</f>
+        <v>91.385729142857102</v>
+      </c>
+      <c r="D6" s="1">
+        <f>_xlfn.STDEV.S(tptday1)</f>
+        <v>0.50088178827996399</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="1">
+        <f>AVERAGE(tptday2)</f>
+        <v>2.1132616571428602</v>
+      </c>
+      <c r="C7" s="1">
+        <f>AVERAGE(tptq2)</f>
+        <v>91.568501428571494</v>
+      </c>
+      <c r="D7" s="1">
+        <f>_xlfn.STDEV.S(tptday2)</f>
+        <v>0.48829660136617897</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="1">
+        <f>AVERAGE(tptday3)</f>
+        <v>2.06589351428571</v>
+      </c>
+      <c r="C8" s="1">
+        <f>AVERAGE(tptq3)</f>
+        <v>91.751638</v>
+      </c>
+      <c r="D8" s="1">
+        <f>_xlfn.STDEV.S(tptday3)</f>
+        <v>0.47734526284924</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="1">
+        <f>AVERAGE(tptday4)</f>
+        <v>2.0414078</v>
+      </c>
+      <c r="C9" s="1">
+        <f>AVERAGE(tptq4)</f>
+        <v>91.935884857142895</v>
+      </c>
+      <c r="D9" s="1">
+        <f>_xlfn.STDEV.S(tptday4)</f>
+        <v>0.479134740416993</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="1">
+        <f>AVERAGE(tptday5)</f>
+        <v>2.0082555714285699</v>
+      </c>
+      <c r="C10" s="1">
+        <f>AVERAGE(tptq5)</f>
+        <v>91.920065714285698</v>
+      </c>
+      <c r="D10" s="1">
+        <f>_xlfn.STDEV.S(tptday5)</f>
+        <v>0.45172107428714697</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="1">
+        <f>AVERAGE(tptday6)</f>
+        <v>1.9535951428571401</v>
+      </c>
+      <c r="C11" s="1">
+        <f>AVERAGE(tptq6)</f>
+        <v>92.303250000000006</v>
+      </c>
+      <c r="D11" s="1">
+        <f>_xlfn.STDEV.S(tptday6)</f>
+        <v>0.453599658167675</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="1">
+        <f>AVERAGE(tptday7)</f>
+        <v>1.91750794285714</v>
+      </c>
+      <c r="C12" s="1">
+        <f>AVERAGE(tptq7)</f>
+        <v>92.464404285714295</v>
+      </c>
+      <c r="D12" s="1">
+        <f>_xlfn.STDEV.S(tptday7)</f>
+        <v>0.42832379122464798</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" s="1">
+        <f>AVERAGE(tptday8)</f>
+        <v>1.87406031428571</v>
+      </c>
+      <c r="C13" s="1">
+        <f>AVERAGE(tptq8)</f>
+        <v>92.661167428571403</v>
+      </c>
+      <c r="D13" s="1">
+        <f>_xlfn.STDEV.S(tptday8)</f>
+        <v>0.42724812134731499</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="1">
+        <f>AVERAGE(tptday9)</f>
+        <v>1.8287006571428599</v>
+      </c>
+      <c r="C14" s="1">
+        <f>AVERAGE(tptq9)</f>
+        <v>92.775435714285706</v>
+      </c>
+      <c r="D14" s="1">
+        <f>_xlfn.STDEV.S(tptday9)</f>
+        <v>0.42837999069496702</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="1">
+        <f>AVERAGE(tptday10)</f>
+        <v>1.79993011428571</v>
+      </c>
+      <c r="C15" s="1">
+        <f>AVERAGE(tptq10)</f>
+        <v>92.957643142857094</v>
+      </c>
+      <c r="D15" s="1">
+        <f>_xlfn.STDEV.S(tptday10)</f>
+        <v>0.40668006493960401</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="1">
+        <f>AVERAGE(tptday11)</f>
+        <v>1.78157377142857</v>
+      </c>
+      <c r="C16" s="1">
+        <f>AVERAGE(tptq11)</f>
+        <v>93.087545428571403</v>
+      </c>
+      <c r="D16" s="1">
+        <f>_xlfn.STDEV.S(tptday11)</f>
+        <v>0.40558788751790897</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="1">
+        <f>AVERAGE(tptday12)</f>
+        <v>1.73122874285714</v>
+      </c>
+      <c r="C17" s="1">
+        <f>AVERAGE(tptq12)</f>
+        <v>93.333743142857102</v>
+      </c>
+      <c r="D17" s="1">
+        <f>_xlfn.STDEV.S(tptday12)</f>
+        <v>0.39691850952692898</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" s="1">
+        <f>AVERAGE(tptday13)</f>
+        <v>1.70249831428571</v>
+      </c>
+      <c r="C18" s="1">
+        <f>AVERAGE(tptq13)</f>
+        <v>93.414434</v>
+      </c>
+      <c r="D18" s="1">
+        <f>_xlfn.STDEV.S(tptday13)</f>
+        <v>0.40283519612541102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="1">
+        <f>AVERAGE(tptday14)</f>
+        <v>1.66465914285714</v>
+      </c>
+      <c r="C19" s="1">
+        <f>AVERAGE(tptq14)</f>
+        <v>93.722237714285697</v>
+      </c>
+      <c r="D19" s="1">
+        <f>_xlfn.STDEV.S(tptday14)</f>
+        <v>0.38255775141509402</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" s="1">
+        <f>AVERAGE(tptday15)</f>
+        <v>1.6370448</v>
+      </c>
+      <c r="C20" s="1">
+        <f>AVERAGE(tptq15)</f>
+        <v>93.696997428571393</v>
+      </c>
+      <c r="D20" s="1">
+        <f>_xlfn.STDEV.S(tptday15)</f>
+        <v>0.37049638868898099</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" s="10">
+        <f>AVERAGE(B6:B20)</f>
+        <v>1.8846869409523801</v>
+      </c>
+      <c r="C21" s="10">
+        <f>AVERAGE(C6:C20)</f>
+        <v>92.598578495238101</v>
+      </c>
+      <c r="D21" s="10">
+        <f>_xlfn.STDEV.S(tptday1)</f>
+        <v>0.50088178827996399</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8457,77 +8747,187 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:27">
-      <c r="A1" s="13" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27">
-      <c r="A3" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-    </row>
-    <row r="4" spans="1:27">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-    </row>
-    <row r="5" spans="1:27">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="11"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="11"/>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="11"/>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="1">
+        <f>AVERAGE(tptday1)</f>
+        <v>2.1506866285714299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="1">
+        <f>AVERAGE(tptday2)</f>
+        <v>2.1132616571428602</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="1">
+        <f>AVERAGE(tptday3)</f>
+        <v>2.06589351428571</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="1">
+        <f>AVERAGE(tptday4)</f>
+        <v>2.0414078</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="1">
+        <f>AVERAGE(tptday5)</f>
+        <v>2.0082555714285699</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="1">
+        <f>AVERAGE(tptday6)</f>
+        <v>1.9535951428571401</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="1">
+        <f>AVERAGE(tptday7)</f>
+        <v>1.91750794285714</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12" s="1">
+        <f>AVERAGE(tptday8)</f>
+        <v>1.87406031428571</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" s="1">
+        <f>AVERAGE(tptday9)</f>
+        <v>1.8287006571428599</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="1">
+        <f>AVERAGE(tptday10)</f>
+        <v>1.79993011428571</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" s="1">
+        <f>AVERAGE(tptday11)</f>
+        <v>1.78157377142857</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="1">
+        <f>AVERAGE(tptday12)</f>
+        <v>1.73122874285714</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" s="1">
+        <f>AVERAGE(tptday13)</f>
+        <v>1.70249831428571</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" s="1">
+        <f>AVERAGE(tptday14)</f>
+        <v>1.66465914285714</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" s="1">
+        <f>AVERAGE(tptday15)</f>
+        <v>1.6370448</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="10">
+        <f>AVERAGE(B5:B19)</f>
+        <v>1.8846869409523801</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8536,80 +8936,27 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:26">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="13" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="3" spans="1:26">
-      <c r="A3" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
-    </row>
-    <row r="4" spans="1:26">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="11"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
-      <c r="Z4" s="11"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -12056,236 +12403,304 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="15.75">
+      <c r="A1" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="11" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="D1" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="B2">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="1">
         <f>AVERAGE(tptday1)</f>
         <v>2.1506866285714299</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <f>AVERAGE(tptq1)</f>
         <v>91.385729142857102</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3">
+      <c r="D2" s="1">
+        <f>_xlfn.STDEV.S(tptday1)</f>
+        <v>0.50088178827996399</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="1">
         <f>AVERAGE(tptday2)</f>
         <v>2.1132616571428602</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <f>AVERAGE(tptq2)</f>
         <v>91.568501428571494</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B4">
+      <c r="D3" s="1">
+        <f>_xlfn.STDEV.S(tptday2)</f>
+        <v>0.48829660136617897</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="1">
         <f>AVERAGE(tptday3)</f>
         <v>2.06589351428571</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <f>AVERAGE(tptq3)</f>
         <v>91.751638</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5">
+      <c r="D4" s="1">
+        <f>_xlfn.STDEV.S(tptday3)</f>
+        <v>0.47734526284924</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="1">
         <f>AVERAGE(tptday4)</f>
         <v>2.0414078</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <f>AVERAGE(tptq4)</f>
         <v>91.935884857142895</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B6">
+      <c r="D5" s="1">
+        <f>_xlfn.STDEV.S(tptday4)</f>
+        <v>0.479134740416993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="1">
         <f>AVERAGE(tptday5)</f>
         <v>2.0082555714285699</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <f>AVERAGE(tptq5)</f>
         <v>91.920065714285698</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B7">
+      <c r="D6" s="1">
+        <f>_xlfn.STDEV.S(tptday5)</f>
+        <v>0.45172107428714697</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="1">
         <f>AVERAGE(tptday6)</f>
         <v>1.9535951428571401</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <f>AVERAGE(tptq6)</f>
         <v>92.303250000000006</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>107</v>
-      </c>
-      <c r="B8">
+      <c r="D7" s="1">
+        <f>_xlfn.STDEV.S(tptday6)</f>
+        <v>0.453599658167675</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="1">
         <f>AVERAGE(tptday7)</f>
         <v>1.91750794285714</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <f>AVERAGE(tptq7)</f>
         <v>92.464404285714295</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B9">
+      <c r="D8" s="1">
+        <f>_xlfn.STDEV.S(tptday7)</f>
+        <v>0.42832379122464798</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="1">
         <f>AVERAGE(tptday8)</f>
         <v>1.87406031428571</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <f>AVERAGE(tptq8)</f>
         <v>92.661167428571403</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>109</v>
-      </c>
-      <c r="B10">
+      <c r="D9" s="1">
+        <f>_xlfn.STDEV.S(tptday8)</f>
+        <v>0.42724812134731499</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="1">
         <f>AVERAGE(tptday9)</f>
         <v>1.8287006571428599</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <f>AVERAGE(tptq9)</f>
         <v>92.775435714285706</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B11">
+      <c r="D10" s="1">
+        <f>_xlfn.STDEV.S(tptday9)</f>
+        <v>0.42837999069496702</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="1">
         <f>AVERAGE(tptday10)</f>
         <v>1.79993011428571</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <f>AVERAGE(tptq10)</f>
         <v>92.957643142857094</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B12">
+      <c r="D11" s="1">
+        <f>_xlfn.STDEV.S(tptday10)</f>
+        <v>0.40668006493960401</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="1">
         <f>AVERAGE(tptday11)</f>
         <v>1.78157377142857</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <f>AVERAGE(tptq11)</f>
         <v>93.087545428571403</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>112</v>
-      </c>
-      <c r="B13">
+      <c r="D12" s="1">
+        <f>_xlfn.STDEV.S(tptday11)</f>
+        <v>0.40558788751790897</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="1">
         <f>AVERAGE(tptday12)</f>
         <v>1.73122874285714</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <f>AVERAGE(tptq12)</f>
         <v>93.333743142857102</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>113</v>
-      </c>
-      <c r="B14">
+      <c r="D13" s="1">
+        <f>_xlfn.STDEV.S(tptday12)</f>
+        <v>0.39691850952692898</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="1">
         <f>AVERAGE(tptday13)</f>
         <v>1.70249831428571</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <f>AVERAGE(tptq13)</f>
         <v>93.414434</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>114</v>
-      </c>
-      <c r="B15">
+      <c r="D14" s="1">
+        <f>_xlfn.STDEV.S(tptday13)</f>
+        <v>0.40283519612541102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" s="1">
         <f>AVERAGE(tptday14)</f>
         <v>1.66465914285714</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <f>AVERAGE(tptq14)</f>
         <v>93.722237714285697</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>115</v>
-      </c>
-      <c r="B16">
+      <c r="D15" s="1">
+        <f>_xlfn.STDEV.S(tptday14)</f>
+        <v>0.38255775141509402</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" s="1">
         <f>AVERAGE(tptday15)</f>
         <v>1.6370448</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <f>AVERAGE(tptq15)</f>
         <v>93.696997428571393</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>116</v>
-      </c>
-      <c r="B17">
+      <c r="D16" s="1">
+        <f>_xlfn.STDEV.S(tptday15)</f>
+        <v>0.37049638868898099</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" s="10">
         <f>AVERAGE(B2:B16)</f>
         <v>1.8846869409523801</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="10">
         <f>AVERAGE(C2:C16)</f>
         <v>92.598578495238101</v>
+      </c>
+      <c r="D17" s="10">
+        <f>_xlfn.STDEV.S(tptday1)</f>
+        <v>0.50088178827996399</v>
       </c>
     </row>
   </sheetData>
@@ -12305,12 +12720,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="11" t="s">
-        <v>117</v>
+      <c r="A2" s="13" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -12324,26 +12739,26 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A3" sqref="A3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
+      <c r="A3" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -12353,29 +12768,29 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -12385,30 +12800,30 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="A1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -12418,30 +12833,30 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="13" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="A1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -12451,26 +12866,26 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="13" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="A1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Made Changes to files and added new ones
</commit_message>
<xml_diff>
--- a/Time&QualityWorkFlow.xlsx
+++ b/Time&QualityWorkFlow.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTOG\DANLC Lab Solution\Anudip-Lab-Solution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609FFB27-2978-41EA-ACC8-486AE2827E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C87040-104C-40F7-947D-79E40E9402D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,6 +69,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -76,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="139">
   <si>
     <t>Day 1</t>
   </si>
@@ -381,6 +383,9 @@
     <t>Average Quality</t>
   </si>
   <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
     <t>Day1</t>
   </si>
   <si>
@@ -429,99 +434,75 @@
     <t>Avg 1to 15</t>
   </si>
   <si>
+    <t xml:space="preserve">Did anyone take more time on Day 15 than Day 14? </t>
+  </si>
+  <si>
     <t>Ans=&gt;NO</t>
   </si>
   <si>
+    <t xml:space="preserve">Did anyone take longer because they were focusing too much on the quality? </t>
+  </si>
+  <si>
     <t>Ans=&gt; Dhruti decrease Quality &amp; Biju &amp; Harshita Increase Quality</t>
   </si>
   <si>
+    <t>How many have shown improvement in terms of TPT on Day 15</t>
+  </si>
+  <si>
     <t>Ans=&gt;Anand,Nupur,Biju,Gopal,Dhanya,Dipa improve quality in Day 15</t>
   </si>
   <si>
+    <t xml:space="preserve">Who are the top 3 members with the lowest TPT on the 15th Day </t>
+  </si>
+  <si>
     <t xml:space="preserve">Ans=&gt;Anushka,Arohi,Firoza members with the lowest TPT on the 15th Day  </t>
   </si>
   <si>
+    <t>who are the top 3 members with the lowest average TPT against day 1 to day 15? Are they the same person?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ans=&gt;Anushka,Arohi,Firoza members with the lowest TPT  against day 1 to  Day 15 </t>
   </si>
   <si>
+    <t>Which charts would give insights for each of the above points?</t>
+  </si>
+  <si>
     <t>Ans=&gt;Line Chart &amp; Column Chart</t>
   </si>
   <si>
-    <t>Ans=&gt;</t>
-  </si>
-  <si>
-    <t>Yes, the average TPT over the last 15 days is 1.867 seconds, which is an improvement compared to the overall average TPT of 1.885 seconds.</t>
-  </si>
-  <si>
-    <t>Yes, the standard deviation of TPT over the last 15 days is 0.150, which is lower than the overall standard deviation of 0.161. This indicates a decrease in variability, meaning the TPT has become more consistent.</t>
-  </si>
-  <si>
-    <t>Yes, the average TPT appears to be gradually decreasing over time from around 2.15.</t>
-  </si>
-  <si>
-    <t>To reduce the TPT further to 1.8, actions such as process optimization, workload balancing, and possibly automation of certain repetitive tasks might be necessary. Additional training or resources could also help to speed up the processes without sacrificing quality.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q1. Did anyone take more time on Day 15 than Day 14? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q2. Did anyone take longer because they were focusing too much on the quality? </t>
-  </si>
-  <si>
-    <t>Q3. How many have shown improvement in terms of TPT on Day 15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q4A. Who are the top 3 members with the lowest TPT on the 15th Day </t>
-  </si>
-  <si>
-    <t>Q4B. Who are the top 3 members with the lowest average TPT against day 1 to day 15? Are they the same person?</t>
-  </si>
-  <si>
-    <t>Q5. Which charts would give insights for each of the above points?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q6. What is the average of TPT against each day? </t>
-  </si>
-  <si>
-    <t>Q1. Did the average TPT improve?</t>
-  </si>
-  <si>
-    <t>Q2. Did the standard deviation decrease over the last 15 days?</t>
-  </si>
-  <si>
-    <t>Q3. Did the average TPT come down from the earlier TPT as your supervisor had indicated? What further actions may be required to bring down the average TPT to 1.8?</t>
-  </si>
-  <si>
-    <t>Q4. What insight would you share on the quality outcomes?</t>
-  </si>
-  <si>
-    <t>Consistency in Time Management: It seems that the time taken did not increase from Day 14 to Day 15, indicating stable process management.</t>
-  </si>
-  <si>
-    <t>Quality vs. Speed Trade-off: Some individuals like Dhruti reduced quality, while others like Biju and Harshit may have taken more time due to focusing on quality. This suggests a potential trade-off between speed and quality that needs to be managed carefully.</t>
+    <t xml:space="preserve">What is the average of TPT against each day? </t>
+  </si>
+  <si>
+    <t>Did the average TPT improve?</t>
+  </si>
+  <si>
+    <t>Ans=&gt;NO,Average TPT Decresed</t>
+  </si>
+  <si>
+    <t>Did the standard deviation decrease over the last 15 days?</t>
+  </si>
+  <si>
+    <t>Ans=&gt;Yes,standard deviation decrease over the last 15 days</t>
+  </si>
+  <si>
+    <t>Did the average TPT come down from the earlier TPT as your supervisor had indicated? What further actions may be required to bring down the average TPT to 1.8?</t>
+  </si>
+  <si>
+    <t>Ans=&gt; Average TPT Already 1.8.  no  further actions may be required to bring down the average TPT to 1.8</t>
+  </si>
+  <si>
+    <t>What insight would you share on the quality outcomes?</t>
+  </si>
+  <si>
+    <t>ANS=&gt; Day 1 to Day 15 Average Quality Increased</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="9">
+  <fonts count="6">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -533,14 +514,15 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -553,21 +535,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -675,37 +649,42 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1050,13 +1029,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>114935</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1103,13 +1082,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1156,13 +1135,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1241,6 +1220,59 @@
         <a:xfrm>
           <a:off x="1193800" y="809625"/>
           <a:ext cx="10893425" cy="6124575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="952500"/>
+          <a:ext cx="13011150" cy="7315200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1517,7 +1549,7 @@
   <dimension ref="A1:BI37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8350,14 +8382,14 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="13" t="s">
-        <v>134</v>
+      <c r="A1" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -8368,87 +8400,345 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="13" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:22">
-      <c r="A1" s="13" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22">
-      <c r="A3" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="5" spans="1:4" ht="15.75">
+      <c r="A5" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="1">
+        <f>AVERAGE(tptday1)</f>
+        <v>2.1506866285714299</v>
+      </c>
+      <c r="C6" s="1">
+        <f>AVERAGE(tptq1)</f>
+        <v>91.385729142857102</v>
+      </c>
+      <c r="D6" s="1">
+        <f>_xlfn.STDEV.S(tptday1)</f>
+        <v>0.50088178827996399</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="1">
+        <f>AVERAGE(tptday2)</f>
+        <v>2.1132616571428602</v>
+      </c>
+      <c r="C7" s="1">
+        <f>AVERAGE(tptq2)</f>
+        <v>91.568501428571494</v>
+      </c>
+      <c r="D7" s="1">
+        <f>_xlfn.STDEV.S(tptday2)</f>
+        <v>0.48829660136617897</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="1">
+        <f>AVERAGE(tptday3)</f>
+        <v>2.06589351428571</v>
+      </c>
+      <c r="C8" s="1">
+        <f>AVERAGE(tptq3)</f>
+        <v>91.751638</v>
+      </c>
+      <c r="D8" s="1">
+        <f>_xlfn.STDEV.S(tptday3)</f>
+        <v>0.47734526284924</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="1">
+        <f>AVERAGE(tptday4)</f>
+        <v>2.0414078</v>
+      </c>
+      <c r="C9" s="1">
+        <f>AVERAGE(tptq4)</f>
+        <v>91.935884857142895</v>
+      </c>
+      <c r="D9" s="1">
+        <f>_xlfn.STDEV.S(tptday4)</f>
+        <v>0.479134740416993</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="1">
+        <f>AVERAGE(tptday5)</f>
+        <v>2.0082555714285699</v>
+      </c>
+      <c r="C10" s="1">
+        <f>AVERAGE(tptq5)</f>
+        <v>91.920065714285698</v>
+      </c>
+      <c r="D10" s="1">
+        <f>_xlfn.STDEV.S(tptday5)</f>
+        <v>0.45172107428714697</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="1">
+        <f>AVERAGE(tptday6)</f>
+        <v>1.9535951428571401</v>
+      </c>
+      <c r="C11" s="1">
+        <f>AVERAGE(tptq6)</f>
+        <v>92.303250000000006</v>
+      </c>
+      <c r="D11" s="1">
+        <f>_xlfn.STDEV.S(tptday6)</f>
+        <v>0.453599658167675</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="1">
+        <f>AVERAGE(tptday7)</f>
+        <v>1.91750794285714</v>
+      </c>
+      <c r="C12" s="1">
+        <f>AVERAGE(tptq7)</f>
+        <v>92.464404285714295</v>
+      </c>
+      <c r="D12" s="1">
+        <f>_xlfn.STDEV.S(tptday7)</f>
+        <v>0.42832379122464798</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" s="1">
+        <f>AVERAGE(tptday8)</f>
+        <v>1.87406031428571</v>
+      </c>
+      <c r="C13" s="1">
+        <f>AVERAGE(tptq8)</f>
+        <v>92.661167428571403</v>
+      </c>
+      <c r="D13" s="1">
+        <f>_xlfn.STDEV.S(tptday8)</f>
+        <v>0.42724812134731499</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="1">
+        <f>AVERAGE(tptday9)</f>
+        <v>1.8287006571428599</v>
+      </c>
+      <c r="C14" s="1">
+        <f>AVERAGE(tptq9)</f>
+        <v>92.775435714285706</v>
+      </c>
+      <c r="D14" s="1">
+        <f>_xlfn.STDEV.S(tptday9)</f>
+        <v>0.42837999069496702</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="1">
+        <f>AVERAGE(tptday10)</f>
+        <v>1.79993011428571</v>
+      </c>
+      <c r="C15" s="1">
+        <f>AVERAGE(tptq10)</f>
+        <v>92.957643142857094</v>
+      </c>
+      <c r="D15" s="1">
+        <f>_xlfn.STDEV.S(tptday10)</f>
+        <v>0.40668006493960401</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="1">
+        <f>AVERAGE(tptday11)</f>
+        <v>1.78157377142857</v>
+      </c>
+      <c r="C16" s="1">
+        <f>AVERAGE(tptq11)</f>
+        <v>93.087545428571403</v>
+      </c>
+      <c r="D16" s="1">
+        <f>_xlfn.STDEV.S(tptday11)</f>
+        <v>0.40558788751790897</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="1">
+        <f>AVERAGE(tptday12)</f>
+        <v>1.73122874285714</v>
+      </c>
+      <c r="C17" s="1">
+        <f>AVERAGE(tptq12)</f>
+        <v>93.333743142857102</v>
+      </c>
+      <c r="D17" s="1">
+        <f>_xlfn.STDEV.S(tptday12)</f>
+        <v>0.39691850952692898</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" s="1">
+        <f>AVERAGE(tptday13)</f>
+        <v>1.70249831428571</v>
+      </c>
+      <c r="C18" s="1">
+        <f>AVERAGE(tptq13)</f>
+        <v>93.414434</v>
+      </c>
+      <c r="D18" s="1">
+        <f>_xlfn.STDEV.S(tptday13)</f>
+        <v>0.40283519612541102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="1">
+        <f>AVERAGE(tptday14)</f>
+        <v>1.66465914285714</v>
+      </c>
+      <c r="C19" s="1">
+        <f>AVERAGE(tptq14)</f>
+        <v>93.722237714285697</v>
+      </c>
+      <c r="D19" s="1">
+        <f>_xlfn.STDEV.S(tptday14)</f>
+        <v>0.38255775141509402</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" s="1">
+        <f>AVERAGE(tptday15)</f>
+        <v>1.6370448</v>
+      </c>
+      <c r="C20" s="1">
+        <f>AVERAGE(tptq15)</f>
+        <v>93.696997428571393</v>
+      </c>
+      <c r="D20" s="1">
+        <f>_xlfn.STDEV.S(tptday15)</f>
+        <v>0.37049638868898099</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" s="10">
+        <f>AVERAGE(B6:B20)</f>
+        <v>1.8846869409523801</v>
+      </c>
+      <c r="C21" s="10">
+        <f>AVERAGE(C6:C20)</f>
+        <v>92.598578495238101</v>
+      </c>
+      <c r="D21" s="10">
+        <f>_xlfn.STDEV.S(tptday1)</f>
+        <v>0.50088178827996399</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8457,77 +8747,187 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:27">
-      <c r="A1" s="13" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27">
-      <c r="A3" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-    </row>
-    <row r="4" spans="1:27">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-    </row>
-    <row r="5" spans="1:27">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="11"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="11"/>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="11"/>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="1">
+        <f>AVERAGE(tptday1)</f>
+        <v>2.1506866285714299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="1">
+        <f>AVERAGE(tptday2)</f>
+        <v>2.1132616571428602</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="1">
+        <f>AVERAGE(tptday3)</f>
+        <v>2.06589351428571</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="1">
+        <f>AVERAGE(tptday4)</f>
+        <v>2.0414078</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="1">
+        <f>AVERAGE(tptday5)</f>
+        <v>2.0082555714285699</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="1">
+        <f>AVERAGE(tptday6)</f>
+        <v>1.9535951428571401</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="1">
+        <f>AVERAGE(tptday7)</f>
+        <v>1.91750794285714</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12" s="1">
+        <f>AVERAGE(tptday8)</f>
+        <v>1.87406031428571</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" s="1">
+        <f>AVERAGE(tptday9)</f>
+        <v>1.8287006571428599</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="1">
+        <f>AVERAGE(tptday10)</f>
+        <v>1.79993011428571</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" s="1">
+        <f>AVERAGE(tptday11)</f>
+        <v>1.78157377142857</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="1">
+        <f>AVERAGE(tptday12)</f>
+        <v>1.73122874285714</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" s="1">
+        <f>AVERAGE(tptday13)</f>
+        <v>1.70249831428571</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" s="1">
+        <f>AVERAGE(tptday14)</f>
+        <v>1.66465914285714</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" s="1">
+        <f>AVERAGE(tptday15)</f>
+        <v>1.6370448</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="10">
+        <f>AVERAGE(B5:B19)</f>
+        <v>1.8846869409523801</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8536,80 +8936,27 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:26">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="13" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="3" spans="1:26">
-      <c r="A3" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
-    </row>
-    <row r="4" spans="1:26">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="11"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
-      <c r="Z4" s="11"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -12056,236 +12403,304 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="15.75">
+      <c r="A1" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="11" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="D1" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="B2">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="1">
         <f>AVERAGE(tptday1)</f>
         <v>2.1506866285714299</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <f>AVERAGE(tptq1)</f>
         <v>91.385729142857102</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3">
+      <c r="D2" s="1">
+        <f>_xlfn.STDEV.S(tptday1)</f>
+        <v>0.50088178827996399</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="1">
         <f>AVERAGE(tptday2)</f>
         <v>2.1132616571428602</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <f>AVERAGE(tptq2)</f>
         <v>91.568501428571494</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B4">
+      <c r="D3" s="1">
+        <f>_xlfn.STDEV.S(tptday2)</f>
+        <v>0.48829660136617897</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="1">
         <f>AVERAGE(tptday3)</f>
         <v>2.06589351428571</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <f>AVERAGE(tptq3)</f>
         <v>91.751638</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5">
+      <c r="D4" s="1">
+        <f>_xlfn.STDEV.S(tptday3)</f>
+        <v>0.47734526284924</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="1">
         <f>AVERAGE(tptday4)</f>
         <v>2.0414078</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <f>AVERAGE(tptq4)</f>
         <v>91.935884857142895</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B6">
+      <c r="D5" s="1">
+        <f>_xlfn.STDEV.S(tptday4)</f>
+        <v>0.479134740416993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="1">
         <f>AVERAGE(tptday5)</f>
         <v>2.0082555714285699</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <f>AVERAGE(tptq5)</f>
         <v>91.920065714285698</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B7">
+      <c r="D6" s="1">
+        <f>_xlfn.STDEV.S(tptday5)</f>
+        <v>0.45172107428714697</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="1">
         <f>AVERAGE(tptday6)</f>
         <v>1.9535951428571401</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <f>AVERAGE(tptq6)</f>
         <v>92.303250000000006</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>107</v>
-      </c>
-      <c r="B8">
+      <c r="D7" s="1">
+        <f>_xlfn.STDEV.S(tptday6)</f>
+        <v>0.453599658167675</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="1">
         <f>AVERAGE(tptday7)</f>
         <v>1.91750794285714</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <f>AVERAGE(tptq7)</f>
         <v>92.464404285714295</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B9">
+      <c r="D8" s="1">
+        <f>_xlfn.STDEV.S(tptday7)</f>
+        <v>0.42832379122464798</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="1">
         <f>AVERAGE(tptday8)</f>
         <v>1.87406031428571</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <f>AVERAGE(tptq8)</f>
         <v>92.661167428571403</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>109</v>
-      </c>
-      <c r="B10">
+      <c r="D9" s="1">
+        <f>_xlfn.STDEV.S(tptday8)</f>
+        <v>0.42724812134731499</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="1">
         <f>AVERAGE(tptday9)</f>
         <v>1.8287006571428599</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <f>AVERAGE(tptq9)</f>
         <v>92.775435714285706</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B11">
+      <c r="D10" s="1">
+        <f>_xlfn.STDEV.S(tptday9)</f>
+        <v>0.42837999069496702</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="1">
         <f>AVERAGE(tptday10)</f>
         <v>1.79993011428571</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <f>AVERAGE(tptq10)</f>
         <v>92.957643142857094</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B12">
+      <c r="D11" s="1">
+        <f>_xlfn.STDEV.S(tptday10)</f>
+        <v>0.40668006493960401</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="1">
         <f>AVERAGE(tptday11)</f>
         <v>1.78157377142857</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <f>AVERAGE(tptq11)</f>
         <v>93.087545428571403</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>112</v>
-      </c>
-      <c r="B13">
+      <c r="D12" s="1">
+        <f>_xlfn.STDEV.S(tptday11)</f>
+        <v>0.40558788751790897</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="1">
         <f>AVERAGE(tptday12)</f>
         <v>1.73122874285714</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <f>AVERAGE(tptq12)</f>
         <v>93.333743142857102</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>113</v>
-      </c>
-      <c r="B14">
+      <c r="D13" s="1">
+        <f>_xlfn.STDEV.S(tptday12)</f>
+        <v>0.39691850952692898</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="1">
         <f>AVERAGE(tptday13)</f>
         <v>1.70249831428571</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <f>AVERAGE(tptq13)</f>
         <v>93.414434</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>114</v>
-      </c>
-      <c r="B15">
+      <c r="D14" s="1">
+        <f>_xlfn.STDEV.S(tptday13)</f>
+        <v>0.40283519612541102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" s="1">
         <f>AVERAGE(tptday14)</f>
         <v>1.66465914285714</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <f>AVERAGE(tptq14)</f>
         <v>93.722237714285697</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>115</v>
-      </c>
-      <c r="B16">
+      <c r="D15" s="1">
+        <f>_xlfn.STDEV.S(tptday14)</f>
+        <v>0.38255775141509402</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" s="1">
         <f>AVERAGE(tptday15)</f>
         <v>1.6370448</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <f>AVERAGE(tptq15)</f>
         <v>93.696997428571393</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>116</v>
-      </c>
-      <c r="B17">
+      <c r="D16" s="1">
+        <f>_xlfn.STDEV.S(tptday15)</f>
+        <v>0.37049638868898099</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" s="10">
         <f>AVERAGE(B2:B16)</f>
         <v>1.8846869409523801</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="10">
         <f>AVERAGE(C2:C16)</f>
         <v>92.598578495238101</v>
+      </c>
+      <c r="D17" s="10">
+        <f>_xlfn.STDEV.S(tptday1)</f>
+        <v>0.50088178827996399</v>
       </c>
     </row>
   </sheetData>
@@ -12305,12 +12720,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="11" t="s">
-        <v>117</v>
+      <c r="A2" s="13" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -12324,26 +12739,26 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A3" sqref="A3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
+      <c r="A3" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -12353,29 +12768,29 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -12385,30 +12800,30 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="A1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -12418,30 +12833,30 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="13" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="A1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -12451,26 +12866,26 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="13" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="A1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>